<commit_message>
DESCW-1270: Multiyear statistics for project change requests tab29
https://apps.itsm.gov.bc.ca/jira/browse/DESCW-1270

* remove Login.tsx
* add Tab_29_rpt_PA_MultiYrStatsChangeRequest.xlsx
* add Tab_29_rpt_PA_MultiYrStatsChangeRequest.js
* add reportSelectorConfig.tsx to include Tab_29_rpt_PA_MultiYrStatsChangeRequest.js
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_29_rpt_PA_MultiYrStatsChangeRequest.xlsx
+++ b/backend/reports/xlsx/Tab_29_rpt_PA_MultiYrStatsChangeRequest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A21F2D95-0CAF-9C4E-86F6-F58748A44EAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB657C35-F84B-8945-800C-935AB767461F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="25600" windowHeight="21100" xr2:uid="{FB9893AD-F19A-BB4E-A83D-FCCFB21F8723}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>{#r=d.report[i]}</t>
   </si>
@@ -50,16 +50,55 @@
     <t>{#date=d.date}</t>
   </si>
   <si>
-    <t>Project #</t>
-  </si>
-  <si>
-    <t>Project Name</t>
-  </si>
-  <si>
     <t>{#fy=d.fiscal_year}</t>
   </si>
   <si>
-    <t>Project ________ for {$fy} as of {$date}</t>
+    <t>Change Request Types for {$fy} as of {$date}</t>
+  </si>
+  <si>
+    <t>FY</t>
+  </si>
+  <si>
+    <t>Total CRs</t>
+  </si>
+  <si>
+    <t>Initiated By</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Schedule</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>{$r.fiscal_year}</t>
+  </si>
+  <si>
+    <t>{$r.cr_count}</t>
+  </si>
+  <si>
+    <t>{$r.initiated_by}</t>
+  </si>
+  <si>
+    <t>{$r.budget}</t>
+  </si>
+  <si>
+    <t>{$r.schedule}</t>
+  </si>
+  <si>
+    <t>{$r.scope}</t>
+  </si>
+  <si>
+    <t>{$r.none}</t>
+  </si>
+  <si>
+    <t>{$r1}</t>
   </si>
 </sst>
 </file>
@@ -87,15 +126,6 @@
       <name val="BCSans-Regular"/>
     </font>
     <font>
-      <sz val="8.5"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="8"/>
-      <name val="BCSans-Regular"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="BCSans-Regular"/>
@@ -103,6 +133,15 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
   </fonts>
@@ -126,27 +165,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FFBFBFBF"/>
-      </left>
-      <right style="medium">
-        <color rgb="FFBFBFBF"/>
-      </right>
-      <top style="medium">
-        <color rgb="FFBFBFBF"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FFBFBFBF"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -201,50 +225,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,8 +287,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1561691</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>145152</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>680356</xdr:rowOff>
     </xdr:to>
@@ -626,109 +635,126 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:B12"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.1640625" customWidth="1"/>
-    <col min="3" max="9" width="15.83203125" customWidth="1"/>
+    <col min="1" max="7" width="14.83203125" customWidth="1"/>
+    <col min="8" max="9" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="57" customHeight="1" thickBot="1">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="15" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A2" s="6" t="s">
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
+      <c r="A4" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" ht="19">
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+    </row>
+    <row r="7" spans="1:9" ht="19">
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="19">
+      <c r="C8" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="19">
+      <c r="C9" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="19">
+      <c r="C10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" ht="19">
+      <c r="C11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A3" s="4"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" ht="20" thickBot="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="7" spans="1:9" ht="19">
-      <c r="B7" s="16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="19">
-      <c r="B8" s="16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="19">
-      <c r="B9" s="16" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="19">
-      <c r="B10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" ht="19">
-      <c r="B11" s="16" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="12" spans="1:9" ht="19">
-      <c r="B12" s="16" t="s">
+      <c r="C12" s="5" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="91" fitToHeight="0" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>